<commit_message>
docs changes from visual studio
</commit_message>
<xml_diff>
--- a/Docs/TestCase Holidays Project.xlsx
+++ b/Docs/TestCase Holidays Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\HolidaysProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\HolidayProjectApp\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BDDCD-CA65-4CF4-B12D-D9A872123DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205A5CDC-B7E0-43FC-B570-C6DFCFCDBD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="368">
   <si>
     <t>ID</t>
   </si>
@@ -1541,6 +1541,9 @@
   </si>
   <si>
     <t>Employee Page</t>
+  </si>
+  <si>
+    <t>TC 069</t>
   </si>
 </sst>
 </file>
@@ -1996,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,6 +4145,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>

</xml_diff>